<commit_message>
void changed to userResponses
</commit_message>
<xml_diff>
--- a/diagrams/endpoints.xlsx
+++ b/diagrams/endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programowanie\Java\automotive-partner-back-end\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8A1A46-426A-4C23-828F-7FE66DD3C704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A672286-F1CC-4C7C-9FF0-AFF745653B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7545" yWindow="7185" windowWidth="14445" windowHeight="10275" xr2:uid="{7C40B4FC-C295-4FDE-BB78-814D8AB719B6}"/>
   </bookViews>
@@ -660,7 +660,7 @@
   <dimension ref="A1:H66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,16 +905,16 @@
       </c>
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -923,21 +923,21 @@
       <c r="F11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -946,21 +946,21 @@
       <c r="F12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="1">
-        <v>0</v>
+      <c r="G12" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -969,21 +969,21 @@
       <c r="F13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -992,8 +992,8 @@
       <c r="F14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="1">
-        <v>0</v>
+      <c r="G14" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
find all blocked and find all unblocked endpoints added
</commit_message>
<xml_diff>
--- a/diagrams/endpoints.xlsx
+++ b/diagrams/endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programowanie\Java\automotive-partner-back-end\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF63862-8A28-4ADA-B562-7C2EBE5FAA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3097CF7B-1453-44BB-87F1-FA2F81C4F7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7545" yWindow="7185" windowWidth="14445" windowHeight="10275" xr2:uid="{7C40B4FC-C295-4FDE-BB78-814D8AB719B6}"/>
   </bookViews>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1555BF42-8AEC-4F54-8DDE-B70EA6966B6F}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,20 +1273,20 @@
         <v>11</v>
       </c>
       <c r="G29" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="B30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -1295,7 +1295,7 @@
       <c r="F30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1323,16 +1323,16 @@
       </c>
     </row>
     <row r="32" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="B32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E32" s="1" t="s">
@@ -1341,7 +1341,7 @@
       <c r="F32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1410,7 +1410,7 @@
       <c r="F35" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G35" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Availability created, two endpoints added
</commit_message>
<xml_diff>
--- a/diagrams/endpoints.xlsx
+++ b/diagrams/endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programowanie\Java\automotive-partner-back-end\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3097CF7B-1453-44BB-87F1-FA2F81C4F7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0005D40A-0756-4C8C-B2FC-D6D234ADCC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7545" yWindow="7185" windowWidth="14445" windowHeight="10275" xr2:uid="{7C40B4FC-C295-4FDE-BB78-814D8AB719B6}"/>
   </bookViews>
@@ -110,9 +110,6 @@
     <t>/api/availability/{user_id}</t>
   </si>
   <si>
-    <t>sumbit</t>
-  </si>
-  <si>
     <t>get_info</t>
   </si>
   <si>
@@ -276,6 +273,9 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>submit</t>
   </si>
 </sst>
 </file>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1555BF42-8AEC-4F54-8DDE-B70EA6966B6F}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +708,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>11</v>
@@ -725,13 +725,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
@@ -754,7 +754,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
@@ -771,13 +771,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -797,10 +797,10 @@
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>14</v>
@@ -823,7 +823,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>14</v>
@@ -840,13 +840,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>14</v>
@@ -869,7 +869,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>14</v>
@@ -886,13 +886,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>14</v>
@@ -915,7 +915,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>14</v>
@@ -932,13 +932,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
@@ -961,7 +961,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>14</v>
@@ -978,19 +978,19 @@
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="G14" s="2">
         <v>2</v>
@@ -1001,10 +1001,10 @@
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>10</v>
@@ -1019,13 +1019,13 @@
         <v>2</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>8</v>
@@ -1034,7 +1034,7 @@
         <v>9</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>14</v>
@@ -1057,7 +1057,7 @@
         <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>11</v>
@@ -1126,7 +1126,7 @@
         <v>17</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>11</v>
@@ -1149,7 +1149,7 @@
         <v>17</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>14</v>
@@ -1172,7 +1172,7 @@
         <v>17</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>14</v>
@@ -1192,10 +1192,10 @@
         <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>14</v>
@@ -1218,7 +1218,7 @@
         <v>17</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>14</v>
@@ -1235,13 +1235,13 @@
         <v>13</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>14</v>
@@ -1255,16 +1255,16 @@
     </row>
     <row r="29" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>14</v>
@@ -1272,91 +1272,91 @@
       <c r="F29" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G29" s="3">
-        <v>3</v>
+      <c r="G29" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="E31" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="1">
-        <v>0</v>
+      <c r="G31" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G32" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>35</v>
+      <c r="B33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>14</v>
@@ -1364,22 +1364,22 @@
       <c r="F33" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G33" s="1">
-        <v>0</v>
+      <c r="G33" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>14</v>
@@ -1393,16 +1393,16 @@
     </row>
     <row r="35" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>14</v>
@@ -1415,25 +1415,25 @@
       </c>
     </row>
     <row r="36" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G36" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1445,7 +1445,7 @@
         <v>8</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>22</v>
@@ -1468,10 +1468,10 @@
         <v>12</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>14</v>
@@ -1488,13 +1488,13 @@
         <v>20</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>14</v>
@@ -1507,16 +1507,16 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="B46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E46" s="1" t="s">
@@ -1525,7 +1525,7 @@
       <c r="F46" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G46" s="1">
+      <c r="G46" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1540,7 +1540,7 @@
         <v>16</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>11</v>
@@ -1553,17 +1553,17 @@
       </c>
     </row>
     <row r="48" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>24</v>
+      <c r="D48" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>11</v>
@@ -1571,8 +1571,8 @@
       <c r="F48" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G48" s="1">
-        <v>0</v>
+      <c r="G48" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1583,10 +1583,10 @@
         <v>12</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>14</v>
@@ -1603,16 +1603,16 @@
     </row>
     <row r="54" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>11</v>
@@ -1626,16 +1626,16 @@
     </row>
     <row r="55" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>11</v>
@@ -1649,16 +1649,16 @@
     </row>
     <row r="56" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>11</v>
@@ -1672,16 +1672,16 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>14</v>
@@ -1695,16 +1695,16 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>14</v>
@@ -1718,16 +1718,16 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>14</v>
@@ -1741,16 +1741,16 @@
     </row>
     <row r="64" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>11</v>
@@ -1764,16 +1764,16 @@
     </row>
     <row r="65" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>11</v>
@@ -1787,16 +1787,16 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="D66" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>14</v>

</xml_diff>